<commit_message>
Final restructuring before golive
</commit_message>
<xml_diff>
--- a/storage/imports/articles.xlsx
+++ b/storage/imports/articles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -28,10 +28,28 @@
     <t>body</t>
   </si>
   <si>
+    <t>bienvenido.jpg</t>
+  </si>
+  <si>
+    <t>Bienvenido</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+  </si>
+  <si>
+    <t>adoptame.jpg</t>
+  </si>
+  <si>
+    <t>Adopcion</t>
+  </si>
+  <si>
+    <t>encontre_o_perdi_mascota.jpg</t>
+  </si>
+  <si>
+    <t>encontre una mascota</t>
+  </si>
+  <si>
     <t>Cuales medios de pago?</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
   </si>
   <si>
     <t>Banner 1</t>
@@ -66,14 +84,24 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,7 +117,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -319,7 +347,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -334,13 +362,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2">
-        <v>13.0</v>
+        <v>21.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -349,11 +380,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B15" si="2">B2</f>
-        <v>13</v>
+        <f t="shared" ref="B3:B4" si="2">B2</f>
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ref="E3:E15" si="3">E2</f>
@@ -367,10 +401,13 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="3"/>
@@ -383,11 +420,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <v>20.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="3"/>
@@ -400,11 +436,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" ref="B6:B15" si="4">B5</f>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="3"/>
@@ -417,11 +453,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="3"/>
@@ -434,11 +470,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="3"/>
@@ -451,11 +487,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="3"/>
@@ -468,11 +504,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="3"/>
@@ -485,11 +521,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="3"/>
@@ -502,11 +538,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="3"/>
@@ -519,11 +555,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="3"/>
@@ -536,11 +572,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="3"/>
@@ -553,11 +589,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="3"/>
@@ -569,10 +605,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="1">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -580,10 +616,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>21.0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18">
@@ -591,10 +627,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
+        <v>21.0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19">
@@ -602,13 +638,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -616,13 +652,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="1">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="str">
-        <f t="shared" ref="E20:E21" si="4">E19</f>
+        <f t="shared" ref="E20:E21" si="5">E19</f>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -631,13 +667,13 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="1">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved migration to a single file
</commit_message>
<xml_diff>
--- a/storage/imports/articles.xlsx
+++ b/storage/imports/articles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -50,15 +50,6 @@
   </si>
   <si>
     <t>Cuales medios de pago?</t>
-  </si>
-  <si>
-    <t>Banner 1</t>
-  </si>
-  <si>
-    <t>Banner 2</t>
-  </si>
-  <si>
-    <t>Banner 3</t>
   </si>
   <si>
     <t>Noticia 1</t>
@@ -74,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -89,6 +80,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -110,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -121,6 +113,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -362,7 +357,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -379,9 +374,8 @@
         <f t="shared" ref="A3:A15" si="1">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <f t="shared" ref="B3:B4" si="2">B2</f>
-        <v>21</v>
+      <c r="B3" s="4">
+        <v>20.0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -390,7 +384,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E15" si="3">E2</f>
+        <f t="shared" ref="E3:E15" si="2">E2</f>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -399,9 +393,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <f t="shared" si="2"/>
-        <v>21</v>
+      <c r="B4" s="4">
+        <v>20.0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -410,7 +403,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -419,14 +412,14 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>20.0</v>
+      <c r="B5" s="4">
+        <v>19.0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -436,14 +429,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B15" si="4">B5</f>
-        <v>20</v>
+        <f t="shared" ref="B6:B15" si="3">B5</f>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -453,14 +446,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -470,14 +463,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -487,14 +480,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -504,14 +497,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -521,14 +514,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -538,14 +531,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -555,14 +548,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -572,14 +565,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
@@ -589,91 +582,58 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="B16" s="4">
         <v>21.0</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E16" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="B17" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B17" s="4">
         <v>21.0</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E17" s="3" t="str">
+        <f t="shared" ref="E17:E18" si="4">E16</f>
+        <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="B18" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="B18" s="4">
         <v>21.0</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="B19" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="3" t="str">
-        <f t="shared" ref="E20:E21" si="5">E19</f>
-        <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="B21" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="3" t="str">
-        <f t="shared" si="5"/>
+      <c r="E18" s="3" t="str">
+        <f t="shared" si="4"/>
         <v>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</v>
       </c>
     </row>

</xml_diff>